<commit_message>
[infra] (Journal de travail): Update du journal de travail
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutSehll\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364EEB72-C169-4F19-811F-5650EE81F6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F296E52-DD72-4011-A286-434C8772A490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">Disscussion avec Mathis quant au projet a faire et les exigences de celui-ci </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place des dossiers/fichiers de travail </t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1167,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0416666666666666E-2</c:v>
+                  <c:v>1.7361111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2139,7 +2142,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 15 minutes</v>
+        <v>0 jours 0 heurs 25 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2158,11 +2161,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2217,15 +2220,23 @@
       <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="str">
+      <c r="A8" s="8">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="47"/>
+        <v>48</v>
+      </c>
+      <c r="B8" s="47">
+        <v>45624</v>
+      </c>
       <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="37"/>
+      <c r="D8" s="49">
+        <v>10</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="M8" t="s">
         <v>3</v>
@@ -8784,7 +8795,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C8" s="29" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8792,7 +8803,7 @@
       </c>
       <c r="D8" s="34">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8847,7 +8858,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9084,6 +9095,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9092,15 +9112,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9123,6 +9134,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9131,12 +9150,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journal de travail): Update journal de travail
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutSehll\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F296E52-DD72-4011-A286-434C8772A490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0F6BFB-E8AE-4A47-97BC-AA85739A28D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mise en place des dossiers/fichiers de travail </t>
+  </si>
+  <si>
+    <t>Mise en place de l'installation de MS teams via le script</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1161,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2089,7 +2092,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2142,7 +2145,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 25 minutes</v>
+        <v>0 jours 1 heurs 25 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2157,7 +2160,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2165,7 +2168,7 @@
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2249,15 +2252,23 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="str">
+      <c r="A9" s="17">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
+        <v>48</v>
+      </c>
+      <c r="B9" s="51">
+        <v>45624</v>
+      </c>
+      <c r="C9" s="52">
+        <v>1</v>
+      </c>
       <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="37"/>
+      <c r="E9" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="18"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -8737,7 +8748,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8749,7 +8760,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8858,7 +8869,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>1.7361111111111112E-2</v>
+        <v>5.9027777777777776E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9095,15 +9106,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9112,6 +9114,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9134,14 +9145,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9150,4 +9153,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journal de travail): Update du journal de travail
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutSehll\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\belkh\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0F6BFB-E8AE-4A47-97BC-AA85739A28D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02BAA40-CD5E-49A6-8550-90ACE32FC897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Mise en place de l'installation de MS teams via le script</t>
+  </si>
+  <si>
+    <t>Mise en place de l'installation de VsCode via le script</t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,81 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -650,154 +727,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1161,7 +1090,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1666666666666664E-2</c:v>
+                  <c:v>4.8611111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1885,18 +1814,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2092,7 +2021,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2145,7 +2074,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 1 heurs 25 minutes</v>
+        <v>0 jours 1 heurs 35 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2164,11 +2093,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2281,15 +2210,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="47"/>
+        <v>48</v>
+      </c>
+      <c r="B10" s="47">
+        <v>45624</v>
+      </c>
       <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="37"/>
+      <c r="D10" s="49">
+        <v>10</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -8625,56 +8562,30 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="E7:E55 E75:E532">
-    <cfRule type="expression" dxfId="24" priority="9">
+  <conditionalFormatting sqref="E7:E532">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56:E74">
-    <cfRule type="expression" dxfId="16" priority="1">
-      <formula>$E56="Autre"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
-      <formula>$E56="Design"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
-      <formula>$E56="Présentation"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
-      <formula>$E56="Meeting"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
-      <formula>$E56="Documentation"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
-      <formula>$E56="Test"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
-      <formula>$E56="Analyse"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
-      <formula>$E56="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -8752,7 +8663,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8760,7 +8671,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>4.1666666666666664E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8869,7 +8780,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>5.9027777777777776E-2</v>
+        <v>6.5972222222222224E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8883,6 +8794,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9105,27 +9036,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9142,23 +9072,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journal de travail ): Update journal de travail
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\belkh\Documents\GitHub\Install_in_NutShell\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02BAA40-CD5E-49A6-8550-90ACE32FC897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD5804D-0A59-48F2-851C-76791869563D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Mise en place de l'installation de VsCode via le script</t>
+  </si>
+  <si>
+    <t>Mise en place de l'installation de docker + ajout dans le groupe docker-user si déjà installé</t>
+  </si>
+  <si>
+    <t>Problème survennue quant a la manière de vérifier si docker est déjà installer, tentative de vérifier si l'installer de docker est présent sur le pc mais cela prenait trop de temps</t>
   </si>
 </sst>
 </file>
@@ -487,80 +493,6 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -727,6 +659,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1090,7 +1096,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8611111111111112E-2</c:v>
+                  <c:v>9.0277777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1814,18 +1820,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2021,7 +2027,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2074,7 +2080,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 1 heurs 35 minutes</v>
+        <v>0 jours 2 heurs 35 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2089,7 +2095,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2097,7 +2103,7 @@
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2238,17 +2244,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="str">
+    <row r="11" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
+        <v>49</v>
+      </c>
+      <c r="B11" s="51">
+        <v>45631</v>
+      </c>
+      <c r="C11" s="52">
+        <v>1</v>
+      </c>
       <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="18"/>
+      <c r="E11" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="M11" t="s">
         <v>6</v>
       </c>
@@ -8563,28 +8579,28 @@
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8659,7 +8675,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8671,7 +8687,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>4.8611111111111112E-2</v>
+        <v>9.0277777777777776E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8780,7 +8796,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>6.5972222222222224E-2</v>
+        <v>0.1076388888888889</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8803,17 +8819,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9036,6 +9041,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9045,17 +9061,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9072,4 +9077,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journaux de travaux): Update journaux de travaux
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD5804D-0A59-48F2-851C-76791869563D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FDB129-B32F-44D0-A907-CF82DF98F2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Problème survennue quant a la manière de vérifier si docker est déjà installer, tentative de vérifier si l'installer de docker est présent sur le pc mais cela prenait trop de temps</t>
+  </si>
+  <si>
+    <t>Mise en place des tests unitaire pour le scipt</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1099,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0277777777777776E-2</c:v>
+                  <c:v>0.1736111111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2027,7 +2030,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2080,7 +2083,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heurs 35 minutes</v>
+        <v>0 jours 4 heurs 35 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2095,7 +2098,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2103,7 +2106,7 @@
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>155</v>
+        <v>275</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2276,15 +2279,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
+        <v>49</v>
+      </c>
+      <c r="B12" s="47">
+        <v>45631</v>
+      </c>
+      <c r="C12" s="48">
+        <v>2</v>
+      </c>
       <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="37"/>
+      <c r="E12" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>35</v>
+      </c>
       <c r="G12" s="16"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -8675,7 +8686,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8687,7 +8698,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>9.0277777777777776E-2</v>
+        <v>0.1736111111111111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8796,7 +8807,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.1076388888888889</v>
+        <v>0.19097222222222221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8810,15 +8821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9041,7 +9043,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9052,15 +9054,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9079,7 +9082,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9088,4 +9091,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journal de travail) update journal de travail
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
+++ b/docs/Journal-de-Travail_BelkhiriaSofiene.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\Install_in_NutShell\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695D6931-E3C4-4C0B-9DC2-68A3C952B47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75068BEB-6BFA-4F3F-9B3E-99D744FBFEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ecriture de la partie développement et conclusion du rapport </t>
+  </si>
+  <si>
+    <t>Mise en place de la plannification &amp; des user stories</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1102,7 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.7361111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.1736111111111111</c:v>
@@ -2033,7 +2036,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2086,7 +2089,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 6 heurs 4 minutes</v>
+        <v>0 jours 6 heurs 30 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2105,11 +2108,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2342,15 +2345,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="47"/>
+        <v>50</v>
+      </c>
+      <c r="B14" s="47">
+        <v>45638</v>
+      </c>
       <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="37"/>
+      <c r="D14" s="49">
+        <v>25</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -8685,7 +8696,7 @@
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C4" s="26" t="str">
         <f>'Journal de travail'!M8</f>
@@ -8693,7 +8704,7 @@
       </c>
       <c r="D4" s="34">
         <f>(A4+B4)/1440</f>
-        <v>0</v>
+        <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -8820,7 +8831,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.25347222222222221</v>
+        <v>0.27083333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9057,15 +9068,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9074,6 +9076,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9096,14 +9107,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9112,4 +9115,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>